<commit_message>
Ajout perf system 1
</commit_message>
<xml_diff>
--- a/EN_319_sources_2020/ressources/Mat_Mult_timing.xlsx
+++ b/EN_319_sources_2020/ressources/Mat_Mult_timing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\EN319-DIM_MAX\EN_319_sources_2020\ressources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A25C45A8-1861-417E-8281-91DE3B11D114}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23BCFB8C-DCBC-4EB3-99CE-5315785B0D89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t>Assciate here a software version with a code snippet for the matrix mulitplication</t>
   </si>
@@ -121,13 +121,22 @@
   </si>
   <si>
     <t>6x6 matrix mult elapsed time(cycles)</t>
+  </si>
+  <si>
+    <t>system_1 (-O3)</t>
+  </si>
+  <si>
+    <t>system_1 (-O0)</t>
+  </si>
+  <si>
+    <t>11</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,6 +147,12 @@
     <font>
       <sz val="11"/>
       <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -241,17 +256,20 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Table!$C$4:$L$4</c:f>
+              <c:f>Table!$C$4:$M$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>144</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
@@ -280,17 +298,20 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Table!$C$5:$L$5</c:f>
+              <c:f>Table!$C$5:$M$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>1.3</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
@@ -319,17 +340,20 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Table!$C$6:$L$6</c:f>
+              <c:f>Table!$C$6:$M$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
@@ -358,17 +382,20 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Table!$C$7:$L$7</c:f>
+              <c:f>Table!$C$7:$M$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>23814</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>1876</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>193</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
@@ -467,7 +494,7 @@
       <xdr:rowOff>33337</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>361950</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
@@ -499,20 +526,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="B1:L7" totalsRowShown="0">
-  <autoFilter ref="B1:L7" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="B1:M7" totalsRowShown="0">
+  <autoFilter ref="B1:M7" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Conf_index"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="1"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="2"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="3"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="4"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="5"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="6"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="7"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="8"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="9"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="10"/>
+    <tableColumn id="13" xr3:uid="{2A8A16EA-4EC0-4CBD-9CA8-B2F05664F234}" name="3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="4"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="5"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="6"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="7"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="8"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="9"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="10"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -839,18 +867,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="180" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="35.28515625" customWidth="1"/>
+    <col min="4" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>11</v>
       </c>
@@ -884,8 +913,11 @@
       <c r="L1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
@@ -893,13 +925,16 @@
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
@@ -912,8 +947,11 @@
       <c r="E3" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>25</v>
       </c>
@@ -921,16 +959,19 @@
         <v>24</v>
       </c>
       <c r="C4">
-        <v>144</v>
+        <v>16</v>
       </c>
       <c r="D4">
+        <v>22</v>
+      </c>
+      <c r="E4">
+        <v>22</v>
+      </c>
+      <c r="F4">
         <v>10</v>
       </c>
-      <c r="E4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" t="s">
         <v>12</v>
@@ -939,13 +980,16 @@
         <v>18</v>
       </c>
       <c r="D5">
+        <v>1.3</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
         <v>10</v>
       </c>
-      <c r="E5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" t="s">
         <v>13</v>
@@ -954,13 +998,16 @@
         <v>20</v>
       </c>
       <c r="D6">
+        <v>1.5</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
         <v>10</v>
       </c>
-      <c r="E6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" t="s">
         <v>29</v>
@@ -969,9 +1016,12 @@
         <v>23814</v>
       </c>
       <c r="D7">
-        <v>10</v>
+        <v>1876</v>
       </c>
       <c r="E7">
+        <v>193</v>
+      </c>
+      <c r="F7">
         <v>10</v>
       </c>
     </row>
@@ -979,6 +1029,7 @@
   <mergeCells count="1">
     <mergeCell ref="A4:A7"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>